<commit_message>
changes done to excel and sales file
</commit_message>
<xml_diff>
--- a/raw_data_cleaned.xlsx
+++ b/raw_data_cleaned.xlsx
@@ -5,27 +5,40 @@
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harsh\OneDrive\Desktop\Sales_Analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harsh\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54D6471B-C6A1-4DE3-9B63-108B5CBBF6CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{040EA3E9-D8E3-4911-A4FD-5C2FE099A053}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{8C418A95-E455-472E-A7FA-38906EDDC306}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8C418A95-E455-472E-A7FA-38906EDDC306}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
     <sheet name="Revenue_by_category" sheetId="3" r:id="rId2"/>
     <sheet name="Revenue_by_region" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames>
+    <definedName name="Slicer_Category">#N/A</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="13" r:id="rId4"/>
+    <pivotCache cacheId="0" r:id="rId4"/>
   </pivotCaches>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{46BE6895-7355-4a93-B00E-2C351335B9C9}">
+      <x15:slicerCaches xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main">
+        <x14:slicerCache r:id="rId5"/>
+      </x15:slicerCaches>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4489" uniqueCount="429">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4503" uniqueCount="443">
   <si>
     <t>OrderID</t>
   </si>
@@ -1314,12 +1327,54 @@
   <si>
     <t xml:space="preserve">Sum of Revenue </t>
   </si>
+  <si>
+    <t>Mean</t>
+  </si>
+  <si>
+    <t>Standard Error</t>
+  </si>
+  <si>
+    <t>Median</t>
+  </si>
+  <si>
+    <t>Mode</t>
+  </si>
+  <si>
+    <t>Standard Deviation</t>
+  </si>
+  <si>
+    <t>Sample Variance</t>
+  </si>
+  <si>
+    <t>Kurtosis</t>
+  </si>
+  <si>
+    <t>Skewness</t>
+  </si>
+  <si>
+    <t>Range</t>
+  </si>
+  <si>
+    <t>Minimum</t>
+  </si>
+  <si>
+    <t>Maximum</t>
+  </si>
+  <si>
+    <t>Sum</t>
+  </si>
+  <si>
+    <t>Count</t>
+  </si>
+  <si>
+    <t>REVENUE</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1450,6 +1505,14 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1636,7 +1699,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -1751,6 +1814,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1796,7 +1879,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1806,7 +1889,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1885,7 +1972,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[raw_data_cleaned_2.xlsx]Revenue_by_category!PivotTable2</c:name>
+    <c:name>[raw_data_cleaned (2).xlsx]Revenue_by_category!PivotTable2</c:name>
     <c:fmtId val="0"/>
   </c:pivotSource>
   <c:chart>
@@ -1940,27 +2027,7 @@
           </a:effectLst>
         </c:spPr>
         <c:marker>
-          <c:symbol val="circle"/>
-          <c:size val="4"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1">
-                <a:lumMod val="60000"/>
-                <a:lumOff val="40000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst>
-              <a:glow rad="63500">
-                <a:schemeClr val="accent1">
-                  <a:satMod val="175000"/>
-                  <a:alpha val="25000"/>
-                </a:schemeClr>
-              </a:glow>
-            </a:effectLst>
-          </c:spPr>
+          <c:symbol val="none"/>
         </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
@@ -2346,7 +2413,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[raw_data_cleaned_2.xlsx]Revenue_by_category!PivotTable2</c:name>
+    <c:name>[raw_data_cleaned (2).xlsx]Revenue_by_category!PivotTable2</c:name>
     <c:fmtId val="12"/>
   </c:pivotSource>
   <c:chart>
@@ -2401,8 +2468,7 @@
           <a:sp3d/>
         </c:spPr>
         <c:marker>
-          <c:symbol val="circle"/>
-          <c:size val="6"/>
+          <c:symbol val="none"/>
         </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
@@ -2467,7 +2533,7 @@
         <c:idx val="1"/>
         <c:spPr>
           <a:solidFill>
-            <a:schemeClr val="accent3"/>
+            <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:ln>
             <a:noFill/>
@@ -2546,6 +2612,44 @@
           </c:extLst>
         </c:dLbl>
       </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="2"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst>
+            <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+              <a:prstClr val="black">
+                <a:alpha val="20000"/>
+              </a:prstClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:sp3d/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="3"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst>
+            <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+              <a:prstClr val="black">
+                <a:alpha val="20000"/>
+              </a:prstClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:sp3d/>
+        </c:spPr>
+      </c:pivotFmt>
     </c:pivotFmts>
     <c:view3D>
       <c:rotX val="50"/>
@@ -2623,6 +2727,11 @@
               </a:effectLst>
               <a:sp3d/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-61FD-4AAB-A4A2-B76A16C81308}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -2643,6 +2752,11 @@
               </a:effectLst>
               <a:sp3d/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-61FD-4AAB-A4A2-B76A16C81308}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -2948,7 +3062,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[raw_data_cleaned_2.xlsx]Revenue_by_region!PivotTable4</c:name>
+    <c:name>[raw_data_cleaned (2).xlsx]Revenue_by_region!PivotTable4</c:name>
     <c:fmtId val="0"/>
   </c:pivotSource>
   <c:chart>
@@ -3031,49 +3145,7 @@
           </a:effectLst>
         </c:spPr>
         <c:marker>
-          <c:symbol val="circle"/>
-          <c:size val="6"/>
-          <c:spPr>
-            <a:gradFill rotWithShape="1">
-              <a:gsLst>
-                <a:gs pos="0">
-                  <a:schemeClr val="accent1">
-                    <a:satMod val="103000"/>
-                    <a:lumMod val="102000"/>
-                    <a:tint val="94000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="50000">
-                  <a:schemeClr val="accent1">
-                    <a:satMod val="110000"/>
-                    <a:lumMod val="100000"/>
-                    <a:shade val="100000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="100000">
-                  <a:schemeClr val="accent1">
-                    <a:lumMod val="99000"/>
-                    <a:satMod val="120000"/>
-                    <a:shade val="78000"/>
-                  </a:schemeClr>
-                </a:gs>
-              </a:gsLst>
-              <a:lin ang="5400000" scaled="0"/>
-            </a:gradFill>
-            <a:ln w="9525">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst>
-              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-                <a:srgbClr val="000000">
-                  <a:alpha val="63000"/>
-                </a:srgbClr>
-              </a:outerShdw>
-            </a:effectLst>
-          </c:spPr>
+          <c:symbol val="none"/>
         </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
@@ -3464,7 +3536,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[raw_data_cleaned_2.xlsx]Revenue_by_region!PivotTable4</c:name>
+    <c:name>[raw_data_cleaned (2).xlsx]Revenue_by_region!PivotTable4</c:name>
     <c:fmtId val="7"/>
   </c:pivotSource>
   <c:chart>
@@ -3548,8 +3620,7 @@
           <a:sp3d/>
         </c:spPr>
         <c:marker>
-          <c:symbol val="circle"/>
-          <c:size val="6"/>
+          <c:symbol val="none"/>
         </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
@@ -3592,6 +3663,174 @@
             <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
           </c:extLst>
         </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="1"/>
+        <c:spPr>
+          <a:gradFill rotWithShape="1">
+            <a:gsLst>
+              <a:gs pos="0">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="103000"/>
+                  <a:lumMod val="102000"/>
+                  <a:tint val="94000"/>
+                </a:schemeClr>
+              </a:gs>
+              <a:gs pos="50000">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="110000"/>
+                  <a:lumMod val="100000"/>
+                  <a:shade val="100000"/>
+                </a:schemeClr>
+              </a:gs>
+              <a:gs pos="100000">
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="99000"/>
+                  <a:satMod val="120000"/>
+                  <a:shade val="78000"/>
+                </a:schemeClr>
+              </a:gs>
+            </a:gsLst>
+            <a:lin ang="5400000" scaled="0"/>
+          </a:gradFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:sp3d/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="2"/>
+        <c:spPr>
+          <a:gradFill rotWithShape="1">
+            <a:gsLst>
+              <a:gs pos="0">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="103000"/>
+                  <a:lumMod val="102000"/>
+                  <a:tint val="94000"/>
+                </a:schemeClr>
+              </a:gs>
+              <a:gs pos="50000">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="110000"/>
+                  <a:lumMod val="100000"/>
+                  <a:shade val="100000"/>
+                </a:schemeClr>
+              </a:gs>
+              <a:gs pos="100000">
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="99000"/>
+                  <a:satMod val="120000"/>
+                  <a:shade val="78000"/>
+                </a:schemeClr>
+              </a:gs>
+            </a:gsLst>
+            <a:lin ang="5400000" scaled="0"/>
+          </a:gradFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:sp3d/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="3"/>
+        <c:spPr>
+          <a:gradFill rotWithShape="1">
+            <a:gsLst>
+              <a:gs pos="0">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="103000"/>
+                  <a:lumMod val="102000"/>
+                  <a:tint val="94000"/>
+                </a:schemeClr>
+              </a:gs>
+              <a:gs pos="50000">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="110000"/>
+                  <a:lumMod val="100000"/>
+                  <a:shade val="100000"/>
+                </a:schemeClr>
+              </a:gs>
+              <a:gs pos="100000">
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="99000"/>
+                  <a:satMod val="120000"/>
+                  <a:shade val="78000"/>
+                </a:schemeClr>
+              </a:gs>
+            </a:gsLst>
+            <a:lin ang="5400000" scaled="0"/>
+          </a:gradFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:sp3d/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="4"/>
+        <c:spPr>
+          <a:gradFill rotWithShape="1">
+            <a:gsLst>
+              <a:gs pos="0">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="103000"/>
+                  <a:lumMod val="102000"/>
+                  <a:tint val="94000"/>
+                </a:schemeClr>
+              </a:gs>
+              <a:gs pos="50000">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="110000"/>
+                  <a:lumMod val="100000"/>
+                  <a:shade val="100000"/>
+                </a:schemeClr>
+              </a:gs>
+              <a:gs pos="100000">
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="99000"/>
+                  <a:satMod val="120000"/>
+                  <a:shade val="78000"/>
+                </a:schemeClr>
+              </a:gs>
+            </a:gsLst>
+            <a:lin ang="5400000" scaled="0"/>
+          </a:gradFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:sp3d/>
+        </c:spPr>
       </c:pivotFmt>
     </c:pivotFmts>
     <c:view3D>
@@ -3694,6 +3933,11 @@
               </a:effectLst>
               <a:sp3d/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-B3EF-4F40-8F07-E81EDBEB166F}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -3737,6 +3981,11 @@
               </a:effectLst>
               <a:sp3d/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-B3EF-4F40-8F07-E81EDBEB166F}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -3780,6 +4029,11 @@
               </a:effectLst>
               <a:sp3d/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-B3EF-4F40-8F07-E81EDBEB166F}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -3823,6 +4077,11 @@
               </a:effectLst>
               <a:sp3d/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-B3EF-4F40-8F07-E81EDBEB166F}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:spPr>
@@ -6349,6 +6608,89 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>685800</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>297180</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>127635</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" Requires="sle15">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="2" name="Category">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2EED1B80-15D9-31BF-074E-6C5D9FB8E528}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2010/slicer">
+              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="Category"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="9700260" y="1691640"/>
+              <a:ext cx="1828800" cy="2466975"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-IN" sz="1100"/>
+                <a:t>This shape represents a table slicer. Table slicers are not supported in this version of Excel.
+If the shape was modified in an earlier version of Excel, or if the workbook was saved in Excel 2007 or earlier, the slicer can't be used.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
@@ -6424,7 +6766,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -18173,7 +18515,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{60AC62B9-B55F-41C2-B9BE-9BA0CF134147}" name="PivotTable2" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="17">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{60AC62B9-B55F-41C2-B9BE-9BA0CF134147}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="17">
   <location ref="A3:B7" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="11">
     <pivotField showAll="0"/>
@@ -18218,7 +18560,7 @@
   <dataFields count="1">
     <dataField name="Sum of Revenue " fld="10" baseField="0" baseItem="0"/>
   </dataFields>
-  <chartFormats count="3">
+  <chartFormats count="5">
     <chartFormat chart="0" format="0" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
@@ -18249,6 +18591,30 @@
         </references>
       </pivotArea>
     </chartFormat>
+    <chartFormat chart="12" format="2">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="6" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="12" format="3">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="6" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
   </chartFormats>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -18263,7 +18629,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A8E71815-8DE5-4CEC-9E75-917B6A57B989}" name="PivotTable4" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="10">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A8E71815-8DE5-4CEC-9E75-917B6A57B989}" name="PivotTable4" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="10">
   <location ref="A3:B8" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="11">
     <pivotField showAll="0"/>
@@ -18312,7 +18678,7 @@
   <dataFields count="1">
     <dataField name="Sum of Revenue " fld="10" baseField="0" baseItem="0"/>
   </dataFields>
-  <chartFormats count="2">
+  <chartFormats count="6">
     <chartFormat chart="0" format="0" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
@@ -18331,6 +18697,54 @@
         </references>
       </pivotArea>
     </chartFormat>
+    <chartFormat chart="7" format="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="4" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="7" format="2">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="4" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="7" format="3">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="4" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="7" format="4">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="4" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
   </chartFormats>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -18344,15 +18758,25 @@
 </pivotTableDefinition>
 </file>
 
+<file path=xl/slicerCaches/slicerCache1.xml><?xml version="1.0" encoding="utf-8"?>
+<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10" name="Slicer_Category" xr10:uid="{B65EBA51-2F01-42DD-99FC-8BC3CEAEFA82}" sourceName="Category">
+  <extLst>
+    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{2F2917AC-EB37-4324-AD4E-5DD8C200BD13}">
+      <x15:tableSlicerCache tableId="1" column="7"/>
+    </x:ext>
+  </extLst>
+</slicerCacheDefinition>
+</file>
+
+<file path=xl/slicers/slicer1.xml><?xml version="1.0" encoding="utf-8"?>
+<slicers xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10">
+  <slicer name="Category" xr10:uid="{E9C13F8B-EF93-4576-93D9-B28158EB4E4A}" cache="Slicer_Category" caption="Category" rowHeight="234950"/>
+</slicers>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C1908F3C-5499-4801-B117-5173F6CAD6D7}" name="Table1" displayName="Table1" ref="A1:K894" totalsRowShown="0">
-  <autoFilter ref="A1:K894" xr:uid="{C1908F3C-5499-4801-B117-5173F6CAD6D7}">
-    <filterColumn colId="4">
-      <customFilters>
-        <customFilter val="**"/>
-      </customFilters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:K894" xr:uid="{C1908F3C-5499-4801-B117-5173F6CAD6D7}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{58A39277-1577-43CC-B516-08FA86E9BA4A}" name="OrderID"/>
     <tableColumn id="2" xr3:uid="{4F2455C5-BAAE-442C-8BEE-75095C1FC82D}" name="OrderDate" dataDxfId="0"/>
@@ -18667,10 +19091,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F399E82-D3A5-4A35-B2AE-C3BCE5C0B84A}">
-  <dimension ref="A1:K894"/>
+  <dimension ref="A1:R894"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="O1" sqref="O1:P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -18686,9 +19110,13 @@
     <col min="11" max="11" width="10.6640625" customWidth="1"/>
     <col min="12" max="12" width="12.5546875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.109375" customWidth="1"/>
+    <col min="16" max="16" width="14.109375" customWidth="1"/>
+    <col min="17" max="17" width="23.6640625" customWidth="1"/>
+    <col min="18" max="18" width="22.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -18723,7 +19151,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1001</v>
       </c>
@@ -18758,7 +19186,7 @@
         <v>2850</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1002</v>
       </c>
@@ -18793,7 +19221,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1003</v>
       </c>
@@ -18828,7 +19256,7 @@
         <v>2380</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1004</v>
       </c>
@@ -18863,7 +19291,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>1005</v>
       </c>
@@ -18898,7 +19326,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1006</v>
       </c>
@@ -18932,8 +19360,12 @@
       <c r="K7">
         <v>510</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="Q7" s="7" t="s">
+        <v>442</v>
+      </c>
+      <c r="R7" s="7"/>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1007</v>
       </c>
@@ -18967,8 +19399,10 @@
       <c r="K8">
         <v>510</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="Q8" s="5"/>
+      <c r="R8" s="5"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1008</v>
       </c>
@@ -19002,8 +19436,14 @@
       <c r="K9">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="Q9" s="5" t="s">
+        <v>429</v>
+      </c>
+      <c r="R9" s="5">
+        <v>1021.4105823068311</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1009</v>
       </c>
@@ -19037,8 +19477,14 @@
       <c r="K10">
         <v>70</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="Q10" s="5" t="s">
+        <v>430</v>
+      </c>
+      <c r="R10" s="5">
+        <v>44.164564872567482</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>1011</v>
       </c>
@@ -19072,8 +19518,14 @@
       <c r="K11">
         <v>1425</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="Q11" s="5" t="s">
+        <v>431</v>
+      </c>
+      <c r="R11" s="5">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>1012</v>
       </c>
@@ -19107,8 +19559,14 @@
       <c r="K12">
         <v>1140</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="Q12" s="5" t="s">
+        <v>432</v>
+      </c>
+      <c r="R12" s="5">
+        <v>1020</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>1013</v>
       </c>
@@ -19142,8 +19600,14 @@
       <c r="K13">
         <v>1800</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="Q13" s="5" t="s">
+        <v>433</v>
+      </c>
+      <c r="R13" s="5">
+        <v>1319.7743556427426</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>1014</v>
       </c>
@@ -19177,8 +19641,14 @@
       <c r="K14">
         <v>600</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="Q14" s="5" t="s">
+        <v>434</v>
+      </c>
+      <c r="R14" s="5">
+        <v>1741804.3498122164</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>1015</v>
       </c>
@@ -19212,8 +19682,14 @@
       <c r="K15">
         <v>4165</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="Q15" s="5" t="s">
+        <v>435</v>
+      </c>
+      <c r="R15" s="5">
+        <v>4.8037968756814529</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>1016</v>
       </c>
@@ -19247,8 +19723,14 @@
       <c r="K16">
         <v>1440</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="Q16" s="5" t="s">
+        <v>436</v>
+      </c>
+      <c r="R16" s="5">
+        <v>2.1144616196032069</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>1017</v>
       </c>
@@ -19282,8 +19764,14 @@
       <c r="K17">
         <v>90</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="Q17" s="5" t="s">
+        <v>437</v>
+      </c>
+      <c r="R17" s="5">
+        <v>6998.2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>1018</v>
       </c>
@@ -19317,8 +19805,14 @@
       <c r="K18">
         <v>1400</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="Q18" s="5" t="s">
+        <v>438</v>
+      </c>
+      <c r="R18" s="5">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>1019</v>
       </c>
@@ -19352,8 +19846,14 @@
       <c r="K19">
         <v>255</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="Q19" s="5" t="s">
+        <v>439</v>
+      </c>
+      <c r="R19" s="5">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>1021</v>
       </c>
@@ -19387,8 +19887,14 @@
       <c r="K20">
         <v>380</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="Q20" s="5" t="s">
+        <v>440</v>
+      </c>
+      <c r="R20" s="5">
+        <v>912119.65000000014</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>1022</v>
       </c>
@@ -19422,8 +19928,14 @@
       <c r="K21">
         <v>95</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="Q21" s="6" t="s">
+        <v>441</v>
+      </c>
+      <c r="R21" s="6">
+        <v>893</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>1023</v>
       </c>
@@ -19458,7 +19970,7 @@
         <v>2295</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>1024</v>
       </c>
@@ -19493,7 +20005,7 @@
         <v>33.25</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>1025</v>
       </c>
@@ -19528,7 +20040,7 @@
         <v>2700</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>1026</v>
       </c>
@@ -19563,7 +20075,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>1027</v>
       </c>
@@ -19598,7 +20110,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>1028</v>
       </c>
@@ -19633,7 +20145,7 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>1029</v>
       </c>
@@ -19668,7 +20180,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>1030</v>
       </c>
@@ -19703,7 +20215,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>1031</v>
       </c>
@@ -19738,7 +20250,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>1032</v>
       </c>
@@ -19773,7 +20285,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>1033</v>
       </c>
@@ -49980,9 +50492,17 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{3A4CF648-6AED-40f4-86FF-DC5316D8AED3}">
+      <x14:slicerList xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main">
+        <x14:slicer r:id="rId3"/>
+      </x14:slicerList>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -50012,7 +50532,7 @@
       <c r="A4" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4">
         <v>770207.5</v>
       </c>
     </row>
@@ -50020,7 +50540,7 @@
       <c r="A5" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5">
         <v>139024</v>
       </c>
     </row>
@@ -50028,7 +50548,7 @@
       <c r="A6" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6">
         <v>2888.15</v>
       </c>
     </row>
@@ -50036,7 +50556,7 @@
       <c r="A7" s="4" t="s">
         <v>427</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7">
         <v>912119.65</v>
       </c>
     </row>
@@ -50050,7 +50570,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{235E35ED-633C-441A-B1A7-B094FF3E989C}">
   <dimension ref="A3:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
@@ -50072,7 +50592,7 @@
       <c r="A4" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4">
         <v>201967.84999999998</v>
       </c>
     </row>
@@ -50080,7 +50600,7 @@
       <c r="A5" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5">
         <v>217840.40000000002</v>
       </c>
     </row>
@@ -50088,7 +50608,7 @@
       <c r="A6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6">
         <v>264748.25</v>
       </c>
     </row>
@@ -50096,7 +50616,7 @@
       <c r="A7" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7">
         <v>227563.15</v>
       </c>
     </row>
@@ -50104,7 +50624,7 @@
       <c r="A8" s="4" t="s">
         <v>427</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8">
         <v>912119.65</v>
       </c>
     </row>

</xml_diff>